<commit_message>
codes for abundance comparison
</commit_message>
<xml_diff>
--- a/data/comparison/merged_16S_verts_wgt.xlsx
+++ b/data/comparison/merged_16S_verts_wgt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaopinghe/Documents/GitHub/offshore_edna/data/comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D00D3D2-68BA-1B49-8933-153B9C5D8828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EFD684-7811-914C-9D8A-2DBC7EDEF58E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="1960" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged_16S_verts_wgt" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="280">
   <si>
     <t>Taxa</t>
   </si>
@@ -777,6 +777,93 @@
   </si>
   <si>
     <t>trawling</t>
+  </si>
+  <si>
+    <t>Alosa_pseudoharengus</t>
+  </si>
+  <si>
+    <t>Amblyraja_radiata</t>
+  </si>
+  <si>
+    <t>Argentina_silus</t>
+  </si>
+  <si>
+    <t>Benthosema_glaciale</t>
+  </si>
+  <si>
+    <t>Centroscyllium_fabricii</t>
+  </si>
+  <si>
+    <t>Citharichthys_arctifrons</t>
+  </si>
+  <si>
+    <t>Clupea_harengus</t>
+  </si>
+  <si>
+    <t>Enchelyopus_cimbrius</t>
+  </si>
+  <si>
+    <t>Glyptocephalus_cynoglossus</t>
+  </si>
+  <si>
+    <t>Helicolenus_dactylopterus</t>
+  </si>
+  <si>
+    <t>Hippoglossus_hippoglossus</t>
+  </si>
+  <si>
+    <t>Leptoclinus_maculatus</t>
+  </si>
+  <si>
+    <t>Leucoraja_erinacea</t>
+  </si>
+  <si>
+    <t>Lophius_americanus</t>
+  </si>
+  <si>
+    <t>Lumpenus_lampretaeformis</t>
+  </si>
+  <si>
+    <t>Melanogrammus_aeglefinus</t>
+  </si>
+  <si>
+    <t>Merluccius_albidus</t>
+  </si>
+  <si>
+    <t>Merluccius_bilinearis</t>
+  </si>
+  <si>
+    <t>Myoxocephalus_octodecemspinosus</t>
+  </si>
+  <si>
+    <t>Notoscopelus_elongatus</t>
+  </si>
+  <si>
+    <t>Phycis_chesteri</t>
+  </si>
+  <si>
+    <t>Pollachius_virens</t>
+  </si>
+  <si>
+    <t>Scomber_scombrus</t>
+  </si>
+  <si>
+    <t>Squalus_acanthias</t>
+  </si>
+  <si>
+    <t>Tautogolabrus_adspersus</t>
+  </si>
+  <si>
+    <t>Triglops_murrayi</t>
+  </si>
+  <si>
+    <t>Urophycis_chuss</t>
+  </si>
+  <si>
+    <t>Urophycis_tenuis</t>
+  </si>
+  <si>
+    <t>Zoarces_americanus</t>
   </si>
 </sst>
 </file>
@@ -32766,7 +32853,7 @@
   <dimension ref="A1:DE31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33105,7 +33192,7 @@
     </row>
     <row r="2" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -33434,7 +33521,7 @@
     </row>
     <row r="3" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>252</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -33763,7 +33850,7 @@
     </row>
     <row r="4" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>253</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -34092,7 +34179,7 @@
     </row>
     <row r="5" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>254</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -34421,7 +34508,7 @@
     </row>
     <row r="6" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -34750,7 +34837,7 @@
     </row>
     <row r="7" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -35079,7 +35166,7 @@
     </row>
     <row r="8" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>257</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -35408,7 +35495,7 @@
     </row>
     <row r="9" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -35737,7 +35824,7 @@
     </row>
     <row r="10" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -36066,7 +36153,7 @@
     </row>
     <row r="11" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>260</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -36395,7 +36482,7 @@
     </row>
     <row r="12" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>261</v>
       </c>
       <c r="B12" s="3">
         <v>3103</v>
@@ -36724,7 +36811,7 @@
     </row>
     <row r="13" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>262</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -37053,7 +37140,7 @@
     </row>
     <row r="14" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>263</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -37382,7 +37469,7 @@
     </row>
     <row r="15" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>264</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -37711,7 +37798,7 @@
     </row>
     <row r="16" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -38040,7 +38127,7 @@
     </row>
     <row r="17" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>266</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -38369,7 +38456,7 @@
     </row>
     <row r="18" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>267</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -38698,7 +38785,7 @@
     </row>
     <row r="19" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>268</v>
       </c>
       <c r="B19" s="3">
         <v>2867</v>
@@ -39027,7 +39114,7 @@
     </row>
     <row r="20" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>269</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -39356,7 +39443,7 @@
     </row>
     <row r="21" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>270</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -39685,7 +39772,7 @@
     </row>
     <row r="22" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>271</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -40014,7 +40101,7 @@
     </row>
     <row r="23" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>272</v>
       </c>
       <c r="B23" s="3">
         <v>6753</v>
@@ -40343,7 +40430,7 @@
     </row>
     <row r="24" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>273</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -41001,7 +41088,7 @@
     </row>
     <row r="26" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>274</v>
       </c>
       <c r="B26" s="3">
         <v>0</v>
@@ -41330,7 +41417,7 @@
     </row>
     <row r="27" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>275</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -41659,7 +41746,7 @@
     </row>
     <row r="28" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>276</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -41988,7 +42075,7 @@
     </row>
     <row r="29" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>277</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -42317,7 +42404,7 @@
     </row>
     <row r="30" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>278</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -42646,7 +42733,7 @@
     </row>
     <row r="31" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>279</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>

</xml_diff>